<commit_message>
fix fonts for all cell to be calibri
</commit_message>
<xml_diff>
--- a/PythonScripts/payment_plan_1.xlsx
+++ b/PythonScripts/payment_plan_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\PythonCreating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soheil izadi\Desktop\TelegramBot\TelegramBot\TelegramBot\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D310F-6487-4A6C-8EB0-E21BAD953BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAD2442-6721-4E50-98D9-5FD371D8672C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1% PP" sheetId="3" r:id="rId1"/>
@@ -258,13 +258,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Tw Cen MT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -275,6 +268,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="21"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,22 +566,19 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,10 +590,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -607,9 +605,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -622,25 +617,31 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1034,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F1C609-B3D0-401B-A2BD-FABD6A9C1BBB}">
   <dimension ref="A4:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,23 +1051,23 @@
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1074,31 +1075,31 @@
         <v>5</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="41">
+      <c r="D9" s="39">
         <f>SUM(D11/80)*100</f>
         <v>1500000</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="49" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="50"/>
-      <c r="D10" s="43">
+      <c r="D10" s="41">
         <v>220213</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="50"/>
-      <c r="D11" s="44">
+      <c r="D11" s="42">
         <v>1200000</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1133,21 +1134,21 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="39"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="15" t="s">
         <v>2</v>
       </c>
@@ -1162,10 +1163,10 @@
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="46"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="3">
         <v>0.1</v>
       </c>
@@ -1181,10 +1182,10 @@
       <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="3">
         <v>0.1</v>
       </c>
@@ -1201,10 +1202,10 @@
       <c r="A19" s="6">
         <v>3</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="7">
         <v>0.01</v>
       </c>
@@ -1221,10 +1222,10 @@
       <c r="A20" s="6">
         <v>4</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="48"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="7">
         <v>0.01</v>
       </c>
@@ -1241,10 +1242,10 @@
       <c r="A21" s="6">
         <v>5</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="7">
         <v>0.01</v>
       </c>
@@ -1261,10 +1262,10 @@
       <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="48"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="7">
         <v>0.01</v>
       </c>
@@ -1281,10 +1282,10 @@
       <c r="A23" s="6">
         <v>7</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="7">
         <v>0.01</v>
       </c>
@@ -1301,10 +1302,10 @@
       <c r="A24" s="6">
         <v>8</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="48"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="7">
         <v>0.01</v>
       </c>
@@ -1321,10 +1322,10 @@
       <c r="A25" s="6">
         <v>9</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="7">
         <v>0.01</v>
       </c>
@@ -1341,10 +1342,10 @@
       <c r="A26" s="9">
         <v>10</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="7">
         <v>0.01</v>
       </c>
@@ -1361,10 +1362,10 @@
       <c r="A27" s="6">
         <v>11</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="48"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="7">
         <v>0.01</v>
       </c>
@@ -1381,10 +1382,10 @@
       <c r="A28" s="6">
         <v>12</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="48"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="7">
         <v>0.01</v>
       </c>
@@ -1401,10 +1402,10 @@
       <c r="A29" s="6">
         <v>13</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="48"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="7">
         <v>0.01</v>
       </c>
@@ -1421,10 +1422,10 @@
       <c r="A30" s="9">
         <v>14</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="48"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="7">
         <v>0.01</v>
       </c>
@@ -1441,10 +1442,10 @@
       <c r="A31" s="6">
         <v>15</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="48"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="7">
         <v>0.01</v>
       </c>
@@ -1461,10 +1462,10 @@
       <c r="A32" s="6">
         <v>16</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="48"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="7">
         <v>0.01</v>
       </c>
@@ -1481,10 +1482,10 @@
       <c r="A33" s="6">
         <v>17</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="48"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="7">
         <v>0.01</v>
       </c>
@@ -1501,10 +1502,10 @@
       <c r="A34" s="9">
         <v>18</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="7">
         <v>0.01</v>
       </c>
@@ -1521,10 +1522,10 @@
       <c r="A35" s="6">
         <v>19</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="7">
         <v>0.01</v>
       </c>
@@ -1541,10 +1542,10 @@
       <c r="A36" s="6">
         <v>20</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="48"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="7">
         <v>0.01</v>
       </c>
@@ -1561,10 +1562,10 @@
       <c r="A37" s="6">
         <v>21</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="48"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="7">
         <v>0.01</v>
       </c>
@@ -1581,10 +1582,10 @@
       <c r="A38" s="9">
         <v>22</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="48"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="7">
         <v>0.01</v>
       </c>
@@ -1601,10 +1602,10 @@
       <c r="A39" s="6">
         <v>23</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="48"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="7">
         <v>0.01</v>
       </c>
@@ -1621,10 +1622,10 @@
       <c r="A40" s="6">
         <v>24</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="48"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="7">
         <v>0.01</v>
       </c>
@@ -1641,10 +1642,10 @@
       <c r="A41" s="6">
         <v>25</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="48"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="7">
         <v>0.01</v>
       </c>
@@ -1661,10 +1662,10 @@
       <c r="A42" s="9">
         <v>26</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="48"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="7">
         <v>0.01</v>
       </c>
@@ -1681,10 +1682,10 @@
       <c r="A43" s="6">
         <v>27</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="48"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="7">
         <v>0.01</v>
       </c>
@@ -1701,10 +1702,10 @@
       <c r="A44" s="6">
         <v>28</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="48"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="7">
         <v>0.01</v>
       </c>
@@ -1721,10 +1722,10 @@
       <c r="A45" s="6">
         <v>33</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="46"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="7">
         <v>0.24</v>
       </c>
@@ -1741,10 +1742,10 @@
       <c r="A46" s="6">
         <v>34</v>
       </c>
-      <c r="B46" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="48"/>
+      <c r="B46" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="27"/>
       <c r="D46" s="7">
         <v>0.01</v>
       </c>
@@ -1761,10 +1762,10 @@
       <c r="A47" s="6">
         <v>35</v>
       </c>
-      <c r="B47" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="48"/>
+      <c r="B47" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="27"/>
       <c r="D47" s="7">
         <v>0.01</v>
       </c>
@@ -1781,10 +1782,10 @@
       <c r="A48" s="9">
         <v>36</v>
       </c>
-      <c r="B48" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="48"/>
+      <c r="B48" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="27"/>
       <c r="D48" s="7">
         <v>0.01</v>
       </c>
@@ -1801,10 +1802,10 @@
       <c r="A49" s="6">
         <v>37</v>
       </c>
-      <c r="B49" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="48"/>
+      <c r="B49" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="27"/>
       <c r="D49" s="7">
         <v>0.01</v>
       </c>
@@ -1821,10 +1822,10 @@
       <c r="A50" s="6">
         <v>38</v>
       </c>
-      <c r="B50" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="48"/>
+      <c r="B50" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="27"/>
       <c r="D50" s="7">
         <v>0.01</v>
       </c>
@@ -1841,10 +1842,10 @@
       <c r="A51" s="6">
         <v>39</v>
       </c>
-      <c r="B51" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="48"/>
+      <c r="B51" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="27"/>
       <c r="D51" s="7">
         <v>0.01</v>
       </c>
@@ -1861,10 +1862,10 @@
       <c r="A52" s="9">
         <v>40</v>
       </c>
-      <c r="B52" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="48"/>
+      <c r="B52" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="27"/>
       <c r="D52" s="7">
         <v>0.01</v>
       </c>
@@ -1881,10 +1882,10 @@
       <c r="A53" s="6">
         <v>41</v>
       </c>
-      <c r="B53" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="48"/>
+      <c r="B53" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="27"/>
       <c r="D53" s="7">
         <v>0.01</v>
       </c>
@@ -1901,10 +1902,10 @@
       <c r="A54" s="6">
         <v>42</v>
       </c>
-      <c r="B54" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="48"/>
+      <c r="B54" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="27"/>
       <c r="D54" s="7">
         <v>0.01</v>
       </c>
@@ -1921,10 +1922,10 @@
       <c r="A55" s="6">
         <v>43</v>
       </c>
-      <c r="B55" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="48"/>
+      <c r="B55" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="27"/>
       <c r="D55" s="7">
         <v>0.01</v>
       </c>
@@ -1941,10 +1942,10 @@
       <c r="A56" s="9">
         <v>44</v>
       </c>
-      <c r="B56" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C56" s="48"/>
+      <c r="B56" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="27"/>
       <c r="D56" s="7">
         <v>0.01</v>
       </c>
@@ -1961,10 +1962,10 @@
       <c r="A57" s="6">
         <v>45</v>
       </c>
-      <c r="B57" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="48"/>
+      <c r="B57" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="27"/>
       <c r="D57" s="7">
         <v>0.01</v>
       </c>
@@ -1981,10 +1982,10 @@
       <c r="A58" s="6">
         <v>46</v>
       </c>
-      <c r="B58" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" s="48"/>
+      <c r="B58" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="27"/>
       <c r="D58" s="7">
         <v>0.01</v>
       </c>
@@ -2001,10 +2002,10 @@
       <c r="A59" s="6">
         <v>47</v>
       </c>
-      <c r="B59" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="48"/>
+      <c r="B59" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="27"/>
       <c r="D59" s="7">
         <v>0.01</v>
       </c>
@@ -2021,10 +2022,10 @@
       <c r="A60" s="9">
         <v>48</v>
       </c>
-      <c r="B60" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="48"/>
+      <c r="B60" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="27"/>
       <c r="D60" s="7">
         <v>0.01</v>
       </c>
@@ -2041,10 +2042,10 @@
       <c r="A61" s="6">
         <v>49</v>
       </c>
-      <c r="B61" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C61" s="48"/>
+      <c r="B61" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="27"/>
       <c r="D61" s="7">
         <v>0.01</v>
       </c>
@@ -2061,10 +2062,10 @@
       <c r="A62" s="6">
         <v>50</v>
       </c>
-      <c r="B62" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="48"/>
+      <c r="B62" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="27"/>
       <c r="D62" s="7">
         <v>0.01</v>
       </c>
@@ -2081,10 +2082,10 @@
       <c r="A63" s="6">
         <v>51</v>
       </c>
-      <c r="B63" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C63" s="48"/>
+      <c r="B63" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="27"/>
       <c r="D63" s="7">
         <v>0.01</v>
       </c>
@@ -2101,10 +2102,10 @@
       <c r="A64" s="9">
         <v>52</v>
       </c>
-      <c r="B64" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="48"/>
+      <c r="B64" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="27"/>
       <c r="D64" s="7">
         <v>0.01</v>
       </c>
@@ -2121,10 +2122,10 @@
       <c r="A65" s="6">
         <v>53</v>
       </c>
-      <c r="B65" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="48"/>
+      <c r="B65" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="27"/>
       <c r="D65" s="7">
         <v>0.01</v>
       </c>
@@ -2141,10 +2142,10 @@
       <c r="A66" s="6">
         <v>54</v>
       </c>
-      <c r="B66" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="48"/>
+      <c r="B66" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="27"/>
       <c r="D66" s="7">
         <v>0.01</v>
       </c>
@@ -2161,10 +2162,10 @@
       <c r="A67" s="6">
         <v>55</v>
       </c>
-      <c r="B67" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="48"/>
+      <c r="B67" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="27"/>
       <c r="D67" s="7">
         <v>0.01</v>
       </c>
@@ -2181,10 +2182,10 @@
       <c r="A68" s="9">
         <v>56</v>
       </c>
-      <c r="B68" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="48"/>
+      <c r="B68" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="27"/>
       <c r="D68" s="7">
         <v>0.01</v>
       </c>
@@ -2201,10 +2202,10 @@
       <c r="A69" s="6">
         <v>57</v>
       </c>
-      <c r="B69" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" s="48"/>
+      <c r="B69" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="27"/>
       <c r="D69" s="7">
         <v>0.01</v>
       </c>
@@ -2221,10 +2222,10 @@
       <c r="A70" s="6">
         <v>58</v>
       </c>
-      <c r="B70" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="48"/>
+      <c r="B70" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="27"/>
       <c r="D70" s="7">
         <v>0.01</v>
       </c>
@@ -2241,10 +2242,10 @@
       <c r="A71" s="6">
         <v>59</v>
       </c>
-      <c r="B71" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71" s="48"/>
+      <c r="B71" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="27"/>
       <c r="D71" s="7">
         <v>0.01</v>
       </c>
@@ -2261,10 +2262,10 @@
       <c r="A72" s="9">
         <v>60</v>
       </c>
-      <c r="B72" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" s="48"/>
+      <c r="B72" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="27"/>
       <c r="D72" s="7">
         <v>0.01</v>
       </c>
@@ -2281,10 +2282,10 @@
       <c r="A73" s="6">
         <v>61</v>
       </c>
-      <c r="B73" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" s="48"/>
+      <c r="B73" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="27"/>
       <c r="D73" s="7">
         <v>0.01</v>
       </c>
@@ -2301,10 +2302,10 @@
       <c r="A74" s="6">
         <v>62</v>
       </c>
-      <c r="B74" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" s="48"/>
+      <c r="B74" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="27"/>
       <c r="D74" s="7">
         <v>0.01</v>
       </c>
@@ -2321,10 +2322,10 @@
       <c r="A75" s="6">
         <v>63</v>
       </c>
-      <c r="B75" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75" s="48"/>
+      <c r="B75" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="27"/>
       <c r="D75" s="7">
         <v>0.01</v>
       </c>
@@ -2338,68 +2339,68 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="33"/>
+      <c r="B76" s="32"/>
       <c r="C76" s="10"/>
       <c r="D76" s="12">
         <f>SUM(D17:D75)</f>
         <v>1.0000000000000004</v>
       </c>
-      <c r="E76" s="34">
+      <c r="E76" s="33">
         <f>SUM(E17:E75)</f>
         <v>0</v>
       </c>
-      <c r="F76" s="35"/>
+      <c r="F76" s="34"/>
     </row>
     <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="38" t="s">
+      <c r="A78" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="40"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="38"/>
     </row>
     <row r="79" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="36" t="s">
+      <c r="A79" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="36"/>
+      <c r="B79" s="35"/>
       <c r="C79" s="6"/>
-      <c r="D79" s="37">
+      <c r="D79" s="36">
         <f>E76</f>
         <v>0</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
     </row>
     <row r="80" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="36" t="s">
+      <c r="A80" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="36"/>
+      <c r="B80" s="35"/>
       <c r="C80" s="6"/>
-      <c r="D80" s="37">
+      <c r="D80" s="36">
         <f>D79*4%</f>
         <v>0</v>
       </c>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
     </row>
     <row r="81" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="36" t="s">
+      <c r="A81" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B81" s="36"/>
+      <c r="B81" s="35"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="37">
+      <c r="D81" s="36">
         <v>4200</v>
       </c>
-      <c r="E81" s="37"/>
-      <c r="F81" s="37"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
     </row>
     <row r="82" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
@@ -2540,33 +2541,95 @@
       <c r="F115" s="19"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="31" t="s">
+      <c r="A116" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="31"/>
-      <c r="C116" s="31"/>
-      <c r="D116" s="31"/>
-      <c r="E116" s="31"/>
-      <c r="F116" s="31"/>
+      <c r="B116" s="30"/>
+      <c r="C116" s="30"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="30"/>
+      <c r="F116" s="30"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="31"/>
-      <c r="B117" s="31"/>
-      <c r="C117" s="31"/>
-      <c r="D117" s="31"/>
-      <c r="E117" s="31"/>
-      <c r="F117" s="31"/>
+      <c r="A117" s="30"/>
+      <c r="B117" s="30"/>
+      <c r="C117" s="30"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="30"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="31"/>
-      <c r="B118" s="31"/>
-      <c r="C118" s="31"/>
-      <c r="D118" s="31"/>
-      <c r="E118" s="31"/>
-      <c r="F118" s="31"/>
+      <c r="A118" s="30"/>
+      <c r="B118" s="30"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
+      <c r="E118" s="30"/>
+      <c r="F118" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="A116:F118"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
@@ -2583,68 +2646,6 @@
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="A116:F118"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>